<commit_message>
update code with latest ggplot2; uses right imports
</commit_message>
<xml_diff>
--- a/inst/extdata/ex01/User_06062018.xlsx
+++ b/inst/extdata/ex01/User_06062018.xlsx
@@ -5,11 +5,11 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profils\mcanouil\Downloads\DATA\endoc_beta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profils\mcanouil\Downloads\DATA\endoc_beta\ex01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="3" r:id="rId1"/>
@@ -49,12 +49,6 @@
     <t>BLANK</t>
   </si>
   <si>
-    <t>SN1</t>
-  </si>
-  <si>
-    <t>SN2</t>
-  </si>
-  <si>
     <t>Sample</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
   </si>
   <si>
     <t>Concentration (µg/L)</t>
-  </si>
-  <si>
-    <t>LYSAT</t>
   </si>
   <si>
     <t>Target</t>
@@ -134,6 +125,15 @@
   </si>
   <si>
     <t>0.5 mM Glc + A</t>
+  </si>
+  <si>
+    <t>LYSATE</t>
+  </si>
+  <si>
+    <t>SUPERNATANT1</t>
+  </si>
+  <si>
+    <t>SUPERNATANT2</t>
   </si>
 </sst>
 </file>
@@ -233,7 +233,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -460,7 +459,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -578,7 +576,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2908,7 +2905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2926,13 +2923,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -2941,19 +2938,19 @@
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2961,10 +2958,10 @@
         <v>43257</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>4</v>
@@ -3194,8 +3191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3220,22 +3217,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>1</v>
@@ -3244,19 +3241,19 @@
         <v>0</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -3277,16 +3274,16 @@
         <v>siNTP</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I2" s="1">
         <v>0.9048581</v>
@@ -3329,16 +3326,16 @@
         <v>siNTP</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1">
         <v>0.84551410000000005</v>
@@ -3381,16 +3378,16 @@
         <v>siNTP</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1">
         <v>0.47709410000000002</v>
@@ -3433,16 +3430,16 @@
         <v>siNTP</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1">
         <v>0.32545099999999999</v>
@@ -3485,16 +3482,16 @@
         <v>siNTP</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1">
         <v>0.41799199999999997</v>
@@ -3537,16 +3534,16 @@
         <v>siNTP</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1">
         <v>0.4046631</v>
@@ -3589,16 +3586,16 @@
         <v>siNTP</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I8">
         <v>0.3388717</v>
@@ -3643,16 +3640,16 @@
         <v>siNTP</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I9">
         <v>0.35027330000000001</v>
@@ -3697,16 +3694,16 @@
         <v>siNTP</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I10">
         <v>0.36398799999999998</v>
@@ -3751,16 +3748,16 @@
         <v>siNTP</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I11">
         <v>0.30241410000000002</v>
@@ -3805,16 +3802,16 @@
         <v>siNTP</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I12">
         <v>0.29688639999999999</v>
@@ -3859,16 +3856,16 @@
         <v>siNTP</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I13">
         <v>0.31960640000000001</v>
@@ -3913,16 +3910,16 @@
         <v>siNTP</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I14" s="1">
         <v>0.3299955</v>
@@ -3967,16 +3964,16 @@
         <v>siNTP</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I15" s="1">
         <v>0.26299479999999997</v>
@@ -4021,16 +4018,16 @@
         <v>siNTP</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I16" s="1">
         <v>0.32744040000000002</v>
@@ -4075,16 +4072,16 @@
         <v>siNTP</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I17" s="1">
         <v>0.82464230000000005</v>
@@ -4129,16 +4126,16 @@
         <v>siNTP</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I18" s="1">
         <v>0.78054979999999996</v>
@@ -4183,16 +4180,16 @@
         <v>siNTP</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I19" s="1">
         <v>1.05976</v>
@@ -4231,7 +4228,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H19"/>
+      <selection activeCell="E2" sqref="E2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4256,22 +4253,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>1</v>
@@ -4280,19 +4277,19 @@
         <v>0</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -4313,16 +4310,16 @@
         <v>siGENE</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I2" s="1">
         <v>0.27928570000000003</v>
@@ -4365,16 +4362,16 @@
         <v>siGENE</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1">
         <v>0.59304579999999996</v>
@@ -4417,16 +4414,16 @@
         <v>siGENE</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1">
         <v>0.2982032</v>
@@ -4469,16 +4466,16 @@
         <v>siGENE</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1">
         <v>0.2879813</v>
@@ -4521,16 +4518,16 @@
         <v>siGENE</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1">
         <v>0.267654</v>
@@ -4573,16 +4570,16 @@
         <v>siGENE</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1">
         <v>0.33135920000000002</v>
@@ -4625,16 +4622,16 @@
         <v>siGENE</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I8">
         <v>0.263797</v>
@@ -4679,16 +4676,16 @@
         <v>siGENE</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I9">
         <v>0.22956480000000001</v>
@@ -4733,16 +4730,16 @@
         <v>siGENE</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I10">
         <v>0.23144609999999999</v>
@@ -4787,16 +4784,16 @@
         <v>siGENE</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I11">
         <v>0.37287310000000001</v>
@@ -4841,16 +4838,16 @@
         <v>siGENE</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I12">
         <v>0.37397249999999999</v>
@@ -4895,16 +4892,16 @@
         <v>siGENE</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I13">
         <v>0.3727896</v>
@@ -4949,16 +4946,16 @@
         <v>siGENE</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I14" s="1">
         <v>0.31245030000000001</v>
@@ -5003,16 +5000,16 @@
         <v>siGENE</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I15" s="1">
         <v>0.2587759</v>
@@ -5057,16 +5054,16 @@
         <v>siGENE</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I16" s="1">
         <v>0.26214890000000002</v>
@@ -5111,16 +5108,16 @@
         <v>siGENE</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I17" s="1">
         <v>0.60261849999999995</v>
@@ -5165,16 +5162,16 @@
         <v>siGENE</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I18" s="1">
         <v>0.50985760000000002</v>
@@ -5219,16 +5216,16 @@
         <v>siGENE</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I19" s="1">
         <v>0.69784299999999999</v>

</xml_diff>